<commit_message>
Finalized Initial Version of Project Plan
</commit_message>
<xml_diff>
--- a/doc/KU4 - Project Plan.xlsx
+++ b/doc/KU4 - Project Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremy\Documents\JeremyBrincat2ndYearProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFC3E9B-F447-47F3-8174-5815042E746F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E6061B7-A03B-4C14-AE64-ED06419709B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43DE01C0-A2D8-4F36-9ADC-E22CC990D539}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>Create an account</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Review datasets</t>
-  </si>
-  <si>
-    <t>Review algorithms</t>
   </si>
   <si>
     <t>Review evaluation metrics</t>
@@ -999,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62287C0-7FD6-48A5-9514-03B257F96545}">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,108 +1008,108 @@
     <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>55</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>56</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>57</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>59</v>
       </c>
-      <c r="R1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="N3" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="O3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="P3" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="Q3" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="R3" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
@@ -1133,7 +1130,8 @@
       <c r="Q4" s="21"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
       <c r="B5" s="11"/>
       <c r="C5" s="1" t="s">
         <v>0</v>
@@ -1154,7 +1152,7 @@
       <c r="Q5" s="20"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
       <c r="C6" s="1" t="s">
         <v>1</v>
@@ -1175,28 +1173,28 @@
       <c r="Q6" s="20"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="11"/>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="26"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="11"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -1215,7 +1213,7 @@
       <c r="Q8" s="20"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>3</v>
       </c>
@@ -1236,7 +1234,8 @@
       <c r="Q9" s="20"/>
       <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
       <c r="B10" s="11"/>
       <c r="C10" s="1" t="s">
         <v>4</v>
@@ -1257,7 +1256,7 @@
       <c r="Q10" s="20"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="11"/>
       <c r="C11" s="1" t="s">
         <v>5</v>
@@ -1278,7 +1277,7 @@
       <c r="Q11" s="20"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="11"/>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -1287,19 +1286,19 @@
       <c r="E12" s="27"/>
       <c r="F12" s="27"/>
       <c r="G12" s="27"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="27"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -1320,7 +1319,7 @@
       <c r="Q13" s="20"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="11"/>
       <c r="C14" s="1" t="s">
         <v>8</v>
@@ -1341,10 +1340,10 @@
       <c r="Q14" s="20"/>
       <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1362,7 +1361,7 @@
       <c r="Q15" s="20"/>
       <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1403,6 +1402,7 @@
       <c r="R17" s="2"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
       <c r="B18" s="11"/>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -1460,7 +1460,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
+      <c r="O20" s="28"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="20"/>
       <c r="R20" s="2"/>
@@ -1473,7 +1473,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1481,7 +1481,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
+      <c r="O21" s="28"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="20"/>
       <c r="R21" s="2"/>
@@ -1502,8 +1502,8 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="28"/>
       <c r="Q22" s="20"/>
       <c r="R22" s="2"/>
     </row>
@@ -1593,7 +1593,7 @@
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="11"/>
       <c r="C27" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1613,9 +1613,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="11"/>
-      <c r="C28" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -1633,7 +1631,9 @@
       <c r="R28" s="2"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
+      <c r="B29" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1652,13 +1652,14 @@
       <c r="R29" s="2"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1677,8 +1678,8 @@
       <c r="C31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
       <c r="F31" s="29"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -1693,16 +1694,16 @@
       <c r="Q31" s="20"/>
       <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="11"/>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="32" t="s">
         <v>64</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1714,19 +1715,19 @@
       <c r="Q32" s="20"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="11"/>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="33" t="s">
         <v>65</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="29"/>
+      <c r="G33" s="1"/>
       <c r="H33" s="29"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -1735,9 +1736,9 @@
       <c r="Q33" s="20"/>
       <c r="R33" s="2"/>
     </row>
-    <row r="34" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B34" s="11"/>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="1"/>
@@ -1745,9 +1746,9 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
       <c r="L34" s="29"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -1758,9 +1759,7 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B35" s="11"/>
-      <c r="C35" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -1778,7 +1777,10 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
+      <c r="A36" s="30"/>
+      <c r="B36" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1797,11 +1799,10 @@
       <c r="R36" s="2"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="1"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1811,7 +1812,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+      <c r="M37" s="30"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
@@ -1832,7 +1833,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
+      <c r="M38" s="30"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -1854,7 +1855,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
-      <c r="N39" s="1"/>
+      <c r="N39" s="30"/>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="20"/>
@@ -1875,7 +1876,7 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
+      <c r="N40" s="30"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="20"/>
@@ -1884,7 +1885,7 @@
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="11"/>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1896,17 +1897,15 @@
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
+      <c r="N41" s="30"/>
+      <c r="O41" s="30"/>
+      <c r="P41" s="30"/>
       <c r="Q41" s="20"/>
       <c r="R41" s="2"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B42" s="11"/>
-      <c r="C42" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -1923,8 +1922,10 @@
       <c r="Q42" s="20"/>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
+    <row r="43" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1942,11 +1943,12 @@
       <c r="Q43" s="20"/>
       <c r="R43" s="2"/>
     </row>
-    <row r="44" spans="1:18" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="s">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="31"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -1958,13 +1960,12 @@
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
+      <c r="O44" s="31"/>
+      <c r="P44" s="31"/>
       <c r="Q44" s="20"/>
       <c r="R44" s="2"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="31"/>
       <c r="B45" s="11"/>
       <c r="C45" s="1" t="s">
         <v>23</v>
@@ -1980,14 +1981,14 @@
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
+      <c r="O45" s="31"/>
+      <c r="P45" s="31"/>
       <c r="Q45" s="20"/>
       <c r="R45" s="2"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="1" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="16" t="s">
         <v>24</v>
       </c>
       <c r="D46" s="1"/>
@@ -2001,50 +2002,29 @@
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
-      <c r="Q46" s="20"/>
-      <c r="R46" s="2"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B47" s="15"/>
-      <c r="C47" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="23"/>
-      <c r="R47" s="17"/>
-    </row>
-    <row r="48" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="13"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="25"/>
-      <c r="Q48" s="24"/>
-      <c r="R48" s="4"/>
+      <c r="O46" s="31"/>
+      <c r="P46" s="31"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="17"/>
+    </row>
+    <row r="47" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="13"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="25"/>
+      <c r="Q47" s="24"/>
+      <c r="R47" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2053,6 +2033,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100504F0EFF1BE61D46A34440DDC749B165" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6861fccdae819c068e3d2675729df3bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="29ddf0ed-477c-451e-8755-cfaffaaa5733" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6fc745dc185d8196f008ac861e10f643" ns2:_="">
     <xsd:import namespace="29ddf0ed-477c-451e-8755-cfaffaaa5733"/>
@@ -2184,12 +2170,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2200,6 +2180,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFD7FEF4-E84B-468B-9D19-73896C646B9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2217,15 +2206,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{58D92219-BA5C-4674-AF14-9AA0F4435448}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FE2ED85-0D3A-4C52-A0D1-D82ED15E39CE}">
   <ds:schemaRefs>

</xml_diff>